<commit_message>
v0.17: fix: search pipeline only checkbox fix: tooltips for long names add: table hover color
</commit_message>
<xml_diff>
--- a/data/UC-1.xlsx
+++ b/data/UC-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\data-metadata\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\data-metadata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954156CB-DF2C-47D2-967B-3C964EDAD838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6116C709-93E1-4F96-BB0E-F1AA7BA6E20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="7460" windowWidth="19130" windowHeight="10610" activeTab="1" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>date_of_birth_of_account_primary_holder_physical_person_date_dt</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CB58EE-03F4-4A2C-B69E-70A0B7A9EECF}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1428,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E77966A-E7E9-4204-A016-12AC6F116326}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1608,7 +1611,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
fills metadata template. lost formatting
</commit_message>
<xml_diff>
--- a/data/UC-1.xlsx
+++ b/data/UC-1.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\data-metadata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6116C709-93E1-4F96-BB0E-F1AA7BA6E20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631EECDA-473C-42B2-AD4E-CB344654AE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
+    <workbookView xWindow="10350" yWindow="5460" windowWidth="23320" windowHeight="11640" activeTab="2" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="TDI GI Pipeline" sheetId="3" r:id="rId2"/>
     <sheet name="ADIDO Metadata" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Adhoc Data-Out" sheetId="6" r:id="rId6"/>
+    <sheet name="Adhoc Data-In" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="95">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>report_1</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -48,9 +49,6 @@
     <t>masked</t>
   </si>
   <si>
-    <t>report_2</t>
-  </si>
-  <si>
     <t>full_name</t>
   </si>
   <si>
@@ -142,6 +140,177 @@
   </si>
   <si>
     <t>date_of_birth_of_account_primary_holder_physical_person_date_dt</t>
+  </si>
+  <si>
+    <t>** A note</t>
+  </si>
+  <si>
+    <t>Data File Name</t>
+  </si>
+  <si>
+    <t>File Type</t>
+  </si>
+  <si>
+    <t>Classification (i.e. Critical, Restricted, Confidential, Internal, Public)</t>
+  </si>
+  <si>
+    <t>Retention Code</t>
+  </si>
+  <si>
+    <t>Retention Period</t>
+  </si>
+  <si>
+    <t>Impacted Jurisdiction Country</t>
+  </si>
+  <si>
+    <t>Impacted Jurisdiction Province</t>
+  </si>
+  <si>
+    <t>Delimiter</t>
+  </si>
+  <si>
+    <t>Line Length</t>
+  </si>
+  <si>
+    <t>**Note</t>
+  </si>
+  <si>
+    <t>Version #</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>AZ-1</t>
+  </si>
+  <si>
+    <t>Data Field Name</t>
+  </si>
+  <si>
+    <t>Field Start Position</t>
+  </si>
+  <si>
+    <t>Field Length</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Team Requesting</t>
+  </si>
+  <si>
+    <t>Sub-Team requesting</t>
+  </si>
+  <si>
+    <t>Also requested by other LOB?</t>
+  </si>
+  <si>
+    <t>New/Existing Initiative</t>
+  </si>
+  <si>
+    <t>Data Out Purpose</t>
+  </si>
+  <si>
+    <t>Type of Data Out</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Process Name</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Recipient Name</t>
+  </si>
+  <si>
+    <t>Contain PII?</t>
+  </si>
+  <si>
+    <t>If External - Please specify 3rd party</t>
+  </si>
+  <si>
+    <t>is the Recipient from another AZ</t>
+  </si>
+  <si>
+    <t>Will it be used in Use-cases?</t>
+  </si>
+  <si>
+    <t>Usecase SME</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>report_2.csv</t>
+  </si>
+  <si>
+    <t>report_1.csv</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Ad-Hoc</t>
+  </si>
+  <si>
+    <t>Proc-1</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>100 days</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Confidential</t>
   </si>
 </sst>
 </file>
@@ -1033,123 +1202,123 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>3</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1158,102 +1327,102 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>3</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
         <v>3</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
         <v>3</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1262,24 +1431,24 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1288,102 +1457,102 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
         <v>3</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
         <v>3</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>3</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1392,24 +1561,24 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1418,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1432,12 +1601,12 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
@@ -1447,177 +1616,177 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>3</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>3</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>3</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1626,21 +1795,21 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1649,11 +1818,456 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083BE9A6-5F21-4A2D-B12D-EDD8B99BB67F}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82028A9A-392C-4B06-A56A-6054FB828DEC}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="A1:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9E1409-1C32-4114-81FF-FEC927A31A2F}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C95133-B435-4363-8B32-DF9DDF66DAE8}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>